<commit_message>
Optimize the display of the results
</commit_message>
<xml_diff>
--- a/Portfolio/GPT_current_holdings.xlsx
+++ b/Portfolio/GPT_current_holdings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiaodong/Library/Mobile Documents/com~apple~CloudDocs/GitHub/AI_stock_analysis_V2/Portfolio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiaodong/Nutstore Files/AIinvest/频道--AI量化对决/Code/LIN-Quantitative-Stock-Selection/Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF75945D-E48A-B640-A9F6-2D83DB536859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE8EA7B-F9FD-DC49-BB44-E5FAB4EB9EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35140" yWindow="2360" windowWidth="28040" windowHeight="17360" xr2:uid="{3F1C265F-C894-CA44-AFDA-40B11C7D779C}"/>
+    <workbookView xWindow="2520" yWindow="500" windowWidth="34560" windowHeight="19720" xr2:uid="{3F1C265F-C894-CA44-AFDA-40B11C7D779C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Cost basis</t>
   </si>
@@ -47,37 +47,31 @@
     <t>Ticker/Cash</t>
   </si>
   <si>
-    <t>PAYC</t>
-  </si>
-  <si>
-    <t>GE</t>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>TOTAL VALUE</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>KLAC</t>
+  </si>
+  <si>
+    <t>HWM</t>
+  </si>
+  <si>
+    <t>PLTR</t>
+  </si>
+  <si>
+    <t>NFLX</t>
   </si>
   <si>
     <t>APH</t>
-  </si>
-  <si>
-    <t>UBER</t>
-  </si>
-  <si>
-    <t>NFLX</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>TOTAL VALUE</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>HWM</t>
-  </si>
-  <si>
-    <t>NVDA</t>
   </si>
 </sst>
 </file>
@@ -452,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69E9176-E15B-3B41-911A-FE13D76F4B54}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="333" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,62 +471,62 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>184</v>
+        <v>630</v>
       </c>
       <c r="C2">
-        <v>570</v>
+        <v>172.2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>621</v>
+        <v>770</v>
       </c>
       <c r="C3">
-        <v>168.85</v>
+        <v>139.6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>1162</v>
+        <v>89</v>
       </c>
       <c r="C4">
-        <v>135.19999999999999</v>
+        <v>1231.5999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>403</v>
+        <v>1884</v>
       </c>
       <c r="C5">
-        <v>255</v>
+        <v>137.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>826</v>
+        <v>448</v>
       </c>
       <c r="C6">
-        <v>78</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -540,51 +534,29 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="C7">
-        <v>1078</v>
+        <v>774.2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>447</v>
+        <v>1730</v>
       </c>
       <c r="C8">
-        <v>234</v>
+        <v>93.6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>1185</v>
-      </c>
-      <c r="C9">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>346</v>
-      </c>
-      <c r="C10">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>30390</v>
+      <c r="D9">
+        <v>7490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>